<commit_message>
added import test for CONFIDENCE.NORM and CONFIDENCE.T, fdo#71350
Change-Id: Id564e201fab17cccaa6b3e9c4353f9f7719345f9
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/functions-excel-2010.xlsx
+++ b/sc/qa/unit/data/xlsx/functions-excel-2010.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\win-docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="14565"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Function</t>
   </si>
@@ -43,6 +48,12 @@
   </si>
   <si>
     <t>F.DIST.RT</t>
+  </si>
+  <si>
+    <t>CONFIDENCE.T</t>
+  </si>
+  <si>
+    <t>CONFIDENCE.NORM</t>
   </si>
 </sst>
 </file>
@@ -104,6 +115,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -151,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -581,6 +595,44 @@
       </c>
       <c r="E8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <f>_xlfn.CONFIDENCE.NORM(C9,D9,E9)</f>
+        <v>1.4935616583311109</v>
+      </c>
+      <c r="C9">
+        <f>2/15</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D9">
+        <v>6.6</v>
+      </c>
+      <c r="E9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <f>_xlfn.CONFIDENCE.NORM(C10,D10,E10)</f>
+        <v>1.4935616583311109</v>
+      </c>
+      <c r="C10">
+        <f>2/15</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D10">
+        <v>6.6</v>
+      </c>
+      <c r="E10">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
round to multiple of absolute significance, fdo#71720 follow-up
The new functions FLOOR.PRECISE, CEILING.PRECISE and ISO.CEILING always
round to a multiple of the absolute value of the significance given,
returning the mathematical floor/ceiling in all cases.

Also changed the test doc to use some meaningful values for these
functions.

Change-Id: Id5a26092838765143e2d308afa49e7119107dac5
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/functions-excel-2010.xlsx
+++ b/sc/qa/unit/data/xlsx/functions-excel-2010.xlsx
@@ -325,9 +325,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -340,6 +337,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,12 +623,12 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="2"/>
+    <col min="1" max="1" width="19.28515625" style="1"/>
     <col min="2" max="2" width="18.28515625"/>
     <col min="3" max="3" width="17.85546875"/>
     <col min="4" max="4" width="8.7109375"/>
@@ -639,1448 +639,1448 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <f>_xlfn.AGGREGATE(F4,1,G2:G10,G6)</f>
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="b">
+      <c r="D2" s="7" t="b">
         <f t="shared" ref="D2:D65" si="0">ROUND(B2,12)=ROUND(C2,12)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="b">
+      <c r="E2" s="7" t="b">
         <f>AND(D2:D73)</f>
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>2</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>44</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <f>_xlfn.BETA.DIST(F2,F5,F5,1,G5,G7)</f>
         <v>0.42284813280246891</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>0.42284813280246902</v>
       </c>
-      <c r="D3" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9">
+      <c r="D3" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
         <v>1.5</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <f>20/15</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>39448</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <f>_xlfn.BETA.DIST(F2,F5,F5,0,G5,G7)</f>
         <v>6.6888842192061565E-2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>6.6888842192061607E-2</v>
       </c>
-      <c r="D4" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
+      <c r="D4" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
         <v>2</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>5</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>39508</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <f>_xlfn.BETA.INV(F5,F5,F6,G5,G7)</f>
         <v>1.0000009059233843</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1.0000009059233801</v>
       </c>
-      <c r="D5" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
+      <c r="D5" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
         <f>2/15</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
         <v>39751</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <f>_xlfn.BINOM.DIST(F6,G2,F5,1)</f>
         <v>1.4317596684776885E-2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>1.43175966847769E-2</v>
       </c>
-      <c r="D6" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
+      <c r="D6" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
         <f>20/15</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>2</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>_xlfn.BINOM.DIST(F6,G2,F5,0)</f>
         <v>1.2474737705548173E-2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>1.2474737705548199E-2</v>
       </c>
-      <c r="D7" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9">
+      <c r="D7" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>6</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <f>_xlfn.BINOM.INV(G2,F5,F5)</f>
         <v>3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9">
+      <c r="D8" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
         <v>2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>6.6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7">
-        <f>_xlfn.CEILING.PRECISE(G6,F5)</f>
+      <c r="B9" s="6">
+        <f>_xlfn.CEILING.PRECISE(F5,G6)</f>
         <v>2</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>2</v>
       </c>
-      <c r="D9" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9">
+      <c r="D9" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <v>4</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7">
-        <f>ISO.CEILING(G6,F5)</f>
+      <c r="B10" s="6">
+        <f>ISO.CEILING(F5,G6)</f>
         <v>2</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>2</v>
       </c>
-      <c r="D10" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9">
+      <c r="D10" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
         <v>2</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <f>_xlfn.CHISQ.DIST(G6,G4,1)</f>
         <v>0.15085496391539036</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0.15085496391538999</v>
       </c>
-      <c r="D11" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="D11" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>_xlfn.CHISQ.DIST.RT(F4,G4)</f>
         <v>0.84914503608460967</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.84914503608461001</v>
       </c>
-      <c r="D12" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="D12" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <f>_xlfn.CHISQ.INV(F5,G4)</f>
         <v>1.8711836505995614</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>1.87118365059956</v>
       </c>
-      <c r="D13" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="D13" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <f>_xlfn.CHISQ.INV.RT(F5,G4)</f>
         <v>8.4454801128564974</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>8.4454801128564991</v>
       </c>
-      <c r="D14" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="D14" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <f>_xlfn.CHISQ.TEST(F2:F10,G2:G10)</f>
         <v>1.8744045912597986E-8</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>1.8744045912597999E-8</v>
       </c>
-      <c r="D15" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f>_xlfn.CONFIDENCE.NORM(F5,G8,G2)</f>
         <v>1.4935616583311109</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>1.49356165833111</v>
       </c>
-      <c r="D16" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="D16" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <f>_xlfn.CONFIDENCE.T(F5,G8,G2)</f>
         <v>1.5223611251194489</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>1.52236112511945</v>
       </c>
-      <c r="D17" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="D17" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <f>_xlfn.COVARIANCE.P(F2:F10,G2:G10)</f>
         <v>2.3040877914951992</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>2.3040877914952</v>
       </c>
-      <c r="D18" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <f>_xlfn.COVARIANCE.S(F2:F10,G2:G10)</f>
         <v>2.5920987654320991</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>2.5920987654320999</v>
       </c>
-      <c r="D19" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <f>_xlfn.ERF.PRECISE(F4)</f>
         <v>0.99532226501895271</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>0.99532226501895305</v>
       </c>
-      <c r="D20" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="D20" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <f>_xlfn.ERFC.PRECISE(F7)</f>
         <v>4.6777349810472645E-3</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>4.6777349810472697E-3</v>
       </c>
-      <c r="D21" s="8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="D21" s="7" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <f>_xlfn.EXPON.DIST(F4,F5,1)</f>
         <v>0.23407166163535131</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>0.23407166163535101</v>
       </c>
-      <c r="D22" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="D22" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <f>_xlfn.EXPON.DIST(F4,F5,0)</f>
         <v>0.10212377844861982</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>0.10212377844861982</v>
       </c>
-      <c r="D23" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="D23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <f>_xlfn.F.DIST(F4,G8,G9,1)</f>
         <v>0.82079999999999997</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>0.82079999999999997</v>
       </c>
-      <c r="D24" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="D24" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <f>_xlfn.F.DIST(F4,G8,G9,0)</f>
         <v>0.1658879999999999</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>0.16588800000000001</v>
       </c>
-      <c r="D25" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="D25" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <f>_xlfn.F.DIST.RT(F4,G4,G7)</f>
         <v>0.21167432749937592</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>0.21167432749937601</v>
       </c>
-      <c r="D26" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="D26" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <f>_xlfn.F.INV(F5,G4,G7)</f>
         <v>0.34789991981862939</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6">
         <v>0.347899919818629</v>
       </c>
-      <c r="D27" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="D27" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <f>_xlfn.F.INV.RT(F5,G4,G7)</f>
         <v>2.652899259689121</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6">
         <v>2.6528992596891201</v>
       </c>
-      <c r="D28" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="D28" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <f>_xlfn.F.TEST(F2:F10,G2:G10)</f>
         <v>5.814996997636946E-8</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>5.81499699763695E-8</v>
       </c>
-      <c r="D29" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="D29" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="7">
-        <f>_xlfn.FLOOR.PRECISE(F4,F5)</f>
-        <v>2</v>
-      </c>
-      <c r="C30" s="7">
-        <v>2</v>
-      </c>
-      <c r="D30" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="B30" s="6">
+        <f>_xlfn.FLOOR.PRECISE(F5,F4)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="D30" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <f>_xlfn.GAMMA.DIST(F2,F5,G5,1)</f>
         <v>0.99207556488413062</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>0.99207556488413096</v>
       </c>
-      <c r="D31" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="D31" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <f>_xlfn.GAMMA.INV(F5,G5,G6)</f>
         <v>0.28620168728134665</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>0.28620168728134698</v>
       </c>
-      <c r="D32" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="D32" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <f>_xlfn.GAMMALN.PRECISE(F4)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="6">
         <v>0</v>
       </c>
-      <c r="D33" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="D33" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <f>_xlfn.HYPGEOM.DIST(G6,G7,G9,G2,1)</f>
         <v>0.93682097822767141</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>0.93682097822767096</v>
       </c>
-      <c r="D34" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="D34" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <f>_xlfn.HYPGEOM.DIST(G6,G7,G9,G2,0)</f>
         <v>0.23364893756272084</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <v>0.23364893756272101</v>
       </c>
-      <c r="D35" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
+      <c r="D35" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <f>_xlfn.LOGNORM.DIST(G4,F8,G8,1)</f>
         <v>0.47640593326077213</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>0.47640593326077202</v>
       </c>
-      <c r="D36" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
+      <c r="D36" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <f>_xlfn.LOGNORM.DIST(G4,F8,G8,0)</f>
         <v>1.2068011575083512E-2</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="6">
         <v>1.20680115750835E-2</v>
       </c>
-      <c r="D37" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
+      <c r="D37" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <f>_xlfn.LOGNORM.INV(F5,G7,G8)</f>
         <v>0.26418843280870008</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>0.26418843280870002</v>
       </c>
-      <c r="D38" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
+      <c r="D38" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="6">
         <f>_xlfn.MODE.MULT(F2:F10)</f>
         <v>2</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="6">
         <v>2</v>
       </c>
-      <c r="D39" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="D39" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="6">
         <f>_xlfn.MODE.SNGL(F2:G10)</f>
         <v>2</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>2</v>
       </c>
-      <c r="D40" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="D40" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="6">
         <f>_xlfn.NEGBINOM.DIST(F4,G4,F5,1)</f>
         <v>6.9952263374485515E-4</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <v>6.9952263374485504E-4</v>
       </c>
-      <c r="D41" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="D41" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="6">
         <f>_xlfn.NEGBINOM.DIST(F4,G4,F5,0)</f>
         <v>4.7477640603566548E-4</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="6">
         <v>4.7477640603566602E-4</v>
       </c>
-      <c r="D42" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="D42" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="6">
         <f>NETWORKDAYS.INTL(H3,H5,1,H4)</f>
         <v>218</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="6">
         <v>218</v>
       </c>
-      <c r="D43" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+      <c r="D43" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="6">
         <f>_xlfn.NORM.DIST(F4,F6,G6,1)</f>
         <v>0.63055865981823644</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="6">
         <v>0.630558659818237</v>
       </c>
-      <c r="D44" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+      <c r="D44" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="6">
         <f>_xlfn.NORM.DIST(F4,F6,G6,0)</f>
         <v>0.18869161384649658</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>0.18869161384649699</v>
       </c>
-      <c r="D45" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="D45" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="6">
         <f>_xlfn.NORM.INV(F5,G3,G6)</f>
         <v>-0.88820989994023836</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="6">
         <v>-0.88820989994023802</v>
       </c>
-      <c r="D46" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+      <c r="D46" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="6">
         <f>_xlfn.NORM.S.DIST(F6,1)</f>
         <v>0.90878878027413212</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>0.90878878027413201</v>
       </c>
-      <c r="D47" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
+      <c r="D47" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="6">
         <f>_xlfn.NORM.S.DIST(F6,0)</f>
         <v>0.16401007467599363</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="6">
         <v>0.16401007467599399</v>
       </c>
-      <c r="D48" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="D48" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="6">
         <f>_xlfn.NORM.S.INV(F5)</f>
         <v>-1.1107716166367858</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>-1.11077161663679</v>
       </c>
-      <c r="D49" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="D49" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="6">
         <f>_xlfn.PERCENTILE.EXC(F2:F10,F5)</f>
         <v>0.53333333333333321</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="6">
         <v>0.53333333333333299</v>
       </c>
-      <c r="D50" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="D50" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="6">
         <f>_xlfn.PERCENTILE.INC(F2:F10,G5)</f>
         <v>4</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>4</v>
       </c>
-      <c r="D51" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="D51" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="6">
         <f>_xlfn.PERCENTILE.EXC(G2:G10,0.1)</f>
         <v>1</v>
       </c>
-      <c r="C52" s="7">
-        <v>1</v>
-      </c>
-      <c r="D52" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+      <c r="C52" s="6">
+        <v>1</v>
+      </c>
+      <c r="D52" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="6">
         <f>_xlfn.PERCENTRANK.INC(F9:G10,G10)</f>
         <v>0</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <v>0</v>
       </c>
-      <c r="D53" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
+      <c r="D53" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="6">
         <f>_xlfn.POISSON.DIST(F6,G6,1)</f>
         <v>0.40600584970983811</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="6">
         <v>0.406005849709838</v>
       </c>
-      <c r="D54" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
+      <c r="D54" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="6">
         <f>_xlfn.POISSON.DIST(F6,G6,0)</f>
         <v>0.27067056647322535</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <v>0.27067056647322502</v>
       </c>
-      <c r="D55" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
+      <c r="D55" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="6">
         <f>_xlfn.QUARTILE.EXC(F2:F10,1)</f>
         <v>1.4166666666666665</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="6">
         <v>1.4166666666666701</v>
       </c>
-      <c r="D56" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
+      <c r="D56" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="6">
         <f>_xlfn.QUARTILE.INC(F2:F10,1)</f>
         <v>1.5</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="6">
         <v>1.5</v>
       </c>
-      <c r="D57" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
+      <c r="D57" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="6">
         <f>_xlfn.RANK.AVG(G6,G2:G9,0)</f>
         <v>6</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="6">
         <v>6</v>
       </c>
-      <c r="D58" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
+      <c r="D58" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="6">
         <f>_xlfn.RANK.EQ(F7,F4,0)</f>
         <v>1</v>
       </c>
-      <c r="C59" s="7">
-        <v>1</v>
-      </c>
-      <c r="D59" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
+      <c r="C59" s="6">
+        <v>1</v>
+      </c>
+      <c r="D59" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="6">
         <f>_xlfn.STDEV.P(F2:F10)</f>
         <v>0.94635246626074987</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="6">
         <v>0.94635246626074998</v>
       </c>
-      <c r="D60" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
+      <c r="D60" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="6">
         <f>_xlfn.STDEV.S(F2:F10)</f>
         <v>1.0037583694283845</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <v>1.00375836942838</v>
       </c>
-      <c r="D61" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
+      <c r="D61" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="6">
         <f>_xlfn.T.DIST(F2,G7,1)</f>
         <v>0.95378684423416238</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="6">
         <v>0.95378684423416304</v>
       </c>
-      <c r="D62" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
+      <c r="D62" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="6">
         <f>_xlfn.T.DIST.2T(F6,G7)</f>
         <v>0.23080940884182113</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <v>0.230809408841821</v>
       </c>
-      <c r="D63" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
+      <c r="D63" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="6">
         <f>_xlfn.T.DIST.RT(F6,G7)</f>
         <v>0.11540470442091057</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="6">
         <v>0.115404704420911</v>
       </c>
-      <c r="D64" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
+      <c r="D64" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="6">
         <f>_xlfn.T.INV(F5,G4)</f>
         <v>-1.2498497882652577</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <v>-1.2498497882652599</v>
       </c>
-      <c r="D65" s="13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
+      <c r="D65" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="6">
         <f>_xlfn.T.INV.2T(F6,G7)</f>
         <v>-0.4527093245918935</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="6">
         <v>-0.452709324591894</v>
       </c>
-      <c r="D66" s="13" t="b">
+      <c r="D66" s="12" t="b">
         <f t="shared" ref="D66:D73" si="1">ROUND(B66,12)=ROUND(C66,12)</f>
         <v>1</v>
       </c>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="6">
         <f>_xlfn.T.TEST(F2:F10,G2:G10,1,1)</f>
         <v>9.4914840602573894E-2</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="6">
         <v>9.4914840602573894E-2</v>
       </c>
-      <c r="D67" s="13" t="b">
+      <c r="D67" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+      <c r="G67" s="8"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="6">
         <f>_xlfn.VAR.P(F2:F10)</f>
         <v>0.89558299039780376</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="6">
         <v>0.89558299039780398</v>
       </c>
-      <c r="D68" s="13" t="b">
+      <c r="D68" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="6">
         <f>_xlfn.VAR.S(F7:F9)</f>
         <v>1.3333333333333339</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="6">
         <v>1.3333333333333299</v>
       </c>
-      <c r="D69" s="13" t="b">
+      <c r="D69" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="6">
         <f>_xlfn.WEIBULL.DIST(F10,F5,G5,1)</f>
         <v>0.66607036427927413</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="6">
         <v>0.66607036427927402</v>
       </c>
-      <c r="D70" s="13" t="b">
+      <c r="D70" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="6">
         <f>_xlfn.WEIBULL.DIST(F10,F5,G5,0)</f>
         <v>2.4417491061254602E-2</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="6">
         <v>2.4417491061254602E-2</v>
       </c>
-      <c r="D71" s="13" t="b">
+      <c r="D71" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="6">
         <f>WORKDAY.INTL(H3,H5,1,H4)</f>
         <v>95099</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <v>95099</v>
       </c>
-      <c r="D72" s="13" t="b">
+      <c r="D72" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="6">
         <f>_xlfn.Z.TEST(F2:F10,G6,F5)</f>
         <v>0.99510746339776501</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>0.99510746339776501</v>
       </c>
-      <c r="D73" s="13" t="b">
+      <c r="D73" s="12" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>